<commit_message>
Added new output collected and generated.
</commit_message>
<xml_diff>
--- a/output/04-26-2023 09-47-54 ingolstadt21 fixed_time_using_TraCI/ingolstadt21_FTSC.xlsx
+++ b/output/04-26-2023 09-47-54 ingolstadt21 fixed_time_using_TraCI/ingolstadt21_FTSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jancy\source\repos\COMPSCI_591_Final_Project\output\04-26-2023 09-47-54 ingolstadt21 fixed_time_using_TraCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FE57250-5B79-4CE9-A90B-A1AA6F94B927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FA47BB-333E-4DF2-AB24-2118F95C2A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6A510252-D67B-4507-A094-AF69F80D054D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6A510252-D67B-4507-A094-AF69F80D054D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingolstadt21_FTSC" sheetId="2" r:id="rId1"/>
@@ -25083,7 +25083,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1493197A-85E0-4662-9011-A67980E3EB52}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="82" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -25422,8 +25422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB2321E-79BE-489F-AB84-775598D6F6F8}">
   <dimension ref="A1:B4001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>